<commit_message>
CHG: updated risk plan with date of last change
</commit_message>
<xml_diff>
--- a/Abschlussdoku/documents/10_risk/RiskManagement.xlsx
+++ b/Abschlussdoku/documents/10_risk/RiskManagement.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23416"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="20740" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Identified</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Alternativen, auf tools verzichten</t>
+  </si>
+  <si>
+    <t>Aktualisierung:</t>
+  </si>
+  <si>
+    <t>Sprint 11: 13.06.2013</t>
   </si>
 </sst>
 </file>
@@ -203,7 +209,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -227,6 +233,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -586,26 +595,32 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="20.7109375" style="1"/>
+    <col min="1" max="1" width="34.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="20.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="20">
       <c r="A1" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -625,7 +640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="42">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -646,7 +661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="42">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -667,7 +682,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="28">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -688,7 +703,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="28">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -709,7 +724,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -730,7 +745,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="28">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -751,7 +766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="42">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -772,7 +787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
@@ -793,7 +808,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>34</v>
       </c>
@@ -814,7 +829,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
@@ -835,7 +850,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="28">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -856,7 +871,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -877,7 +892,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="28">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
@@ -898,7 +913,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="28">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -939,7 +954,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -956,7 +971,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>